<commit_message>
created test for VPE Assignment; removed Add Topic VPE as duplicate
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP Trunk\src\main\resources\keywords.metadata\metadata\staging\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8093BD1F-88BF-477D-AFBE-9C356C906FD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28245" windowHeight="12660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -247,6 +241,9 @@
     <t>BUILDEMPIREADMINURL</t>
   </si>
   <si>
+    <t>https://admin.staging.bppdigital.buildempire.app</t>
+  </si>
+  <si>
     <t>STAGINGVLENOCASLOGINURL</t>
   </si>
   <si>
@@ -262,12 +259,18 @@
     <t>BUILDEMPIREBESPOKEURL</t>
   </si>
   <si>
+    <t>https://staging.bppdigital.buildempire.app/account?registration_type=rbs</t>
+  </si>
+  <si>
     <t>BUILDEMPIRELOGINURL</t>
   </si>
   <si>
     <t>BUILDEMPIRECHANNELISLANDURL</t>
   </si>
   <si>
+    <t>https://staging.bppdigital.buildempire.app/account?registration_type=jersey</t>
+  </si>
+  <si>
     <t>BPPDIGITALINSIGHTSURL</t>
   </si>
   <si>
@@ -329,22 +332,19 @@
   </si>
   <si>
     <t>CREDITCARDCVV</t>
-  </si>
-  <si>
-    <t>https://admin.staging.bppdigital.buildempire.app</t>
-  </si>
-  <si>
-    <t>https://staging.bppdigital.buildempire.app/account?registration_type=jersey</t>
-  </si>
-  <si>
-    <t>https://staging.bppdigital.buildempire.app/account?registration_type=rbs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,8 +381,144 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,8 +531,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -419,10 +741,249 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -436,45 +997,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -732,27 +1336,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.71428571428571" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" style="13" customWidth="1"/>
-    <col min="2" max="2" width="45.42578125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="13"/>
+    <col min="1" max="1" width="33.8571428571429" style="14" customWidth="1"/>
+    <col min="2" max="2" width="45.4285714285714" style="14" customWidth="1"/>
+    <col min="3" max="3" width="44.1428571428571" style="14" customWidth="1"/>
+    <col min="4" max="16384" width="8.71428571428571" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -764,315 +1368,317 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="16" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B11" r:id="rId4" tooltip="mailto:neilsteward@outlook.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId1" display="Abcd1234@"/>
+    <hyperlink ref="B7" r:id="rId2" display="apprenticeships@bpptest.com"/>
+    <hyperlink ref="B9" r:id="rId3" display="waltdisney@mailinator.com"/>
+    <hyperlink ref="B11" r:id="rId4" display="neilsteward@outlook.com" tooltip="mailto:neilsteward@outlook.com"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="26.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1091,7 +1697,7 @@
       <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1132,24 +1738,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="52.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="52.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="26.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1233,8 +1841,8 @@
       <c r="A8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>102</v>
+      <c r="B8" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1242,42 +1850,42 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1286,114 +1894,116 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="B3" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" tooltip="https://staging.bppdigital.buildempire.app/account" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="B9" r:id="rId7" tooltip="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="B12" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="B8" r:id="rId10" xr:uid="{D106736D-D69E-4416-9667-2242F2E61EDA}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{3041DC18-D6EE-4A90-9332-6BADD93DF56F}"/>
-    <hyperlink ref="B11" r:id="rId12" xr:uid="{147EE7FB-61B8-4A85-A91D-114ECCE1B072}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://landdportal-stage.bpp.com/auth/saml/login.php"/>
+    <hyperlink ref="B6" r:id="rId2" display="https://trainthetutor-stage.bpp.com/login/index.php"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://cod-stage.bpp.com/login/index.php"/>
+    <hyperlink ref="B4" r:id="rId4" display="https://study-stage.bpp.com/login/index.php"/>
+    <hyperlink ref="B3" r:id="rId5" display="https://lms-stage.bpp.com/login/index.php"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://staging.bppdigital.buildempire.app/account" tooltip="https://staging.bppdigital.buildempire.app/account"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS" tooltip="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS"/>
+    <hyperlink ref="B10" r:id="rId8" display="http://bpp-stage.apolloglobal.int/openbravo"/>
+    <hyperlink ref="B12" r:id="rId6" display="https://staging.bppdigital.buildempire.app/account"/>
+    <hyperlink ref="B8" r:id="rId9" display="https://admin.staging.bppdigital.buildempire.app"/>
+    <hyperlink ref="B13" r:id="rId10" display="https://staging.bppdigital.buildempire.app/account?registration_type=jersey"/>
+    <hyperlink ref="B11" r:id="rId11" display="https://staging.bppdigital.buildempire.app/account?registration_type=rbs"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="34.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="37.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1409,10 +2019,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1420,10 +2030,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1431,10 +2041,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1442,7 +2052,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B5" s="3">
         <v>10</v>
@@ -1453,10 +2063,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B6" s="3">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1464,7 +2074,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B7" s="3">
         <v>737</v>
@@ -1474,6 +2084,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>